<commit_message>
Completed structure of code. Completed smooth round detail calculations.
</commit_message>
<xml_diff>
--- a/db/smooth_round.xlsx
+++ b/db/smooth_round.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yarovii/GitHub/aratta/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA2FC44-C63B-AC42-A367-556153D028AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F57D67-FAC9-B841-8160-04E0FFE8D8BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8520" yWindow="460" windowWidth="20220" windowHeight="16540" xr2:uid="{EDFD01D9-7D40-444D-82A2-723E98B2746A}"/>
   </bookViews>
@@ -531,14 +531,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF9FC98-6BA8-C848-A88D-249B6FE68355}">
   <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
       <c r="B1" s="1">
         <v>140</v>
       </c>

</xml_diff>